<commit_message>
code 1811 - 10
</commit_message>
<xml_diff>
--- a/ui/data/test_execution_list.xlsx
+++ b/ui/data/test_execution_list.xlsx
@@ -16,39 +16,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>test_add_address</t>
+  </si>
+  <si>
+    <t>TC_Name</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>test_edit_address</t>
+  </si>
+  <si>
+    <t>test_login</t>
+  </si>
+  <si>
+    <t>test_register_user</t>
+  </si>
+  <si>
+    <t>test_search</t>
+  </si>
+  <si>
+    <t>Sno</t>
+  </si>
+  <si>
+    <t>TC_path</t>
+  </si>
+  <si>
+    <t>./ui/tests/test_add_address.py</t>
+  </si>
+  <si>
+    <t>./ui/tests/test_search.py</t>
+  </si>
+  <si>
+    <t>./ui/tests/registration/test_registration.py</t>
+  </si>
+  <si>
+    <t>./ui/tests/test_login.py</t>
+  </si>
   <si>
     <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>test_add_address</t>
-  </si>
-  <si>
-    <t>TC_Name</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Run</t>
-  </si>
-  <si>
-    <t>test_edit_address</t>
-  </si>
-  <si>
-    <t>test_login</t>
-  </si>
-  <si>
-    <t>test_register_user</t>
-  </si>
-  <si>
-    <t>test_search</t>
-  </si>
-  <si>
-    <t>Sno</t>
   </si>
 </sst>
 </file>
@@ -419,90 +434,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3"/>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3"/>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
code 1811 - 03
</commit_message>
<xml_diff>
--- a/ui/data/test_execution_list.xlsx
+++ b/ui/data/test_execution_list.xlsx
@@ -437,7 +437,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -489,7 +489,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -534,7 +534,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E6" s="3"/>
     </row>

</xml_diff>

<commit_message>
code 1811 - 05
</commit_message>
<xml_diff>
--- a/ui/data/test_execution_list.xlsx
+++ b/ui/data/test_execution_list.xlsx
@@ -489,7 +489,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -504,7 +504,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3"/>
     </row>

</xml_diff>

<commit_message>
code 1811 - 07
</commit_message>
<xml_diff>
--- a/ui/data/test_execution_list.xlsx
+++ b/ui/data/test_execution_list.xlsx
@@ -437,7 +437,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -474,7 +474,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E2" s="3"/>
     </row>
@@ -489,7 +489,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -519,7 +519,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E5" s="3"/>
     </row>

</xml_diff>

<commit_message>
code 1811 - 11
</commit_message>
<xml_diff>
--- a/ui/data/test_execution_list.xlsx
+++ b/ui/data/test_execution_list.xlsx
@@ -437,7 +437,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -474,7 +474,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E2" s="3"/>
     </row>
@@ -489,7 +489,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -534,7 +534,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E6" s="3"/>
     </row>

</xml_diff>